<commit_message>
Integrated Curing Calculations with the main GELxy software
</commit_message>
<xml_diff>
--- a/Curing Calculations Data.xlsx
+++ b/Curing Calculations Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yushrajkapoor/Desktop/NauenLab/GELxy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4D7B079-5480-5848-863D-9C7A4932EBEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7259EF7-0037-2449-89AE-17002CB9CDE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="17280" yWindow="760" windowWidth="17280" windowHeight="21580" xr2:uid="{EB474C7A-A58E-EB45-A49F-20C7A37E07CB}"/>
   </bookViews>
@@ -422,7 +422,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19:R19"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Update to Curing Calculations Data Rohan has collected some data points which has enabled an update to the Curing Calculations Data excel spreadsheet
</commit_message>
<xml_diff>
--- a/Curing Calculations Data.xlsx
+++ b/Curing Calculations Data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yushrajkapoor/Desktop/NauenLab/GELxy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C93D27AE-AA0C-7D48-B560-93E60D8EBC32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04801EDA-EAF6-934A-9C1C-6817A105BBE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="17280" yWindow="760" windowWidth="17280" windowHeight="21580" xr2:uid="{EB474C7A-A58E-EB45-A49F-20C7A37E07CB}"/>
   </bookViews>
@@ -41,13 +41,13 @@
     <t>Beam Diameter (mm)</t>
   </si>
   <si>
-    <t>Stiffness (kPa)</t>
-  </si>
-  <si>
     <t>Velocity (mm/s)</t>
   </si>
   <si>
     <t>Current (mA)</t>
+  </si>
+  <si>
+    <t>Stiffness (Pa)</t>
   </si>
 </sst>
 </file>
@@ -419,10 +419,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE870D1B-018D-334B-BFEA-83AC63CF19E9}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -441,13 +441,13 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -455,13 +455,88 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>100</v>
+        <v>8100</v>
       </c>
       <c r="C2">
-        <v>0.1</v>
+        <v>9.9999999999999992E-25</v>
       </c>
       <c r="D2">
-        <v>0.1</v>
+        <v>2755.13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>8100</v>
+      </c>
+      <c r="C3">
+        <f>1/(5*60)</f>
+        <v>3.3333333333333335E-3</v>
+      </c>
+      <c r="D3">
+        <v>4431.4399999999996</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>8100</v>
+      </c>
+      <c r="C4">
+        <f>1/(10*60)</f>
+        <v>1.6666666666666668E-3</v>
+      </c>
+      <c r="D4">
+        <v>7661.76</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>8100</v>
+      </c>
+      <c r="C5">
+        <f>1/(15*60)</f>
+        <v>1.1111111111111111E-3</v>
+      </c>
+      <c r="D5">
+        <v>8860.2000000000007</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>3</v>
+      </c>
+      <c r="B6">
+        <v>8100</v>
+      </c>
+      <c r="C6">
+        <f>1/(20*60)</f>
+        <v>8.3333333333333339E-4</v>
+      </c>
+      <c r="D6">
+        <v>10619.1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>3</v>
+      </c>
+      <c r="B7">
+        <v>8100</v>
+      </c>
+      <c r="C7">
+        <f>1/(25*60)</f>
+        <v>6.6666666666666664E-4</v>
+      </c>
+      <c r="D7">
+        <v>12749.44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix to bug where the baseline stiffness (time=0) had a low velocity, but it should've had an infinite value. But since increasing this to infinity (or any bery high number) would break the calculations, I decided to omit this data point
</commit_message>
<xml_diff>
--- a/Curing Calculations Data.xlsx
+++ b/Curing Calculations Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yushrajkapoor/Desktop/NauenLab/GELxy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04801EDA-EAF6-934A-9C1C-6817A105BBE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{761A6A5E-C598-C94F-BAA8-06A82CAAF557}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17280" yWindow="760" windowWidth="17280" windowHeight="21580" xr2:uid="{EB474C7A-A58E-EB45-A49F-20C7A37E07CB}"/>
+    <workbookView xWindow="8440" yWindow="760" windowWidth="26120" windowHeight="21580" xr2:uid="{EB474C7A-A58E-EB45-A49F-20C7A37E07CB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -54,7 +54,14 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -80,14 +87,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -100,6 +110,940 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="38100" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="log"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$2:$C$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>9999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.0000000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.3333333333333335E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.5000000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$2:$D$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>2755.13</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4431.4399999999996</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7661.76</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8860.2000000000007</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10619.1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12749.44</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-0D4A-7D4A-B47A-419CBD0BF8E0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="402355520"/>
+        <c:axId val="402357232"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="402355520"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="402357232"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="402357232"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="402355520"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>137160</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>40640</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>411480</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>142240</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D5927BA3-4FF8-448A-A853-81301D2F8B39}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -419,10 +1363,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE870D1B-018D-334B-BFEA-83AC63CF19E9}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -458,7 +1402,7 @@
         <v>8100</v>
       </c>
       <c r="C2">
-        <v>9.9999999999999992E-25</v>
+        <v>9999</v>
       </c>
       <c r="D2">
         <v>2755.13</v>
@@ -472,8 +1416,8 @@
         <v>8100</v>
       </c>
       <c r="C3">
-        <f>1/(5*60)</f>
-        <v>3.3333333333333335E-3</v>
+        <f>3/(5*60)</f>
+        <v>0.01</v>
       </c>
       <c r="D3">
         <v>4431.4399999999996</v>
@@ -487,8 +1431,8 @@
         <v>8100</v>
       </c>
       <c r="C4">
-        <f>1/(10*60)</f>
-        <v>1.6666666666666668E-3</v>
+        <f>3/(10*60)</f>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="D4">
         <v>7661.76</v>
@@ -502,8 +1446,8 @@
         <v>8100</v>
       </c>
       <c r="C5">
-        <f>1/(15*60)</f>
-        <v>1.1111111111111111E-3</v>
+        <f>3/(15*60)</f>
+        <v>3.3333333333333335E-3</v>
       </c>
       <c r="D5">
         <v>8860.2000000000007</v>
@@ -517,8 +1461,8 @@
         <v>8100</v>
       </c>
       <c r="C6">
-        <f>1/(20*60)</f>
-        <v>8.3333333333333339E-4</v>
+        <f>3/(20*60)</f>
+        <v>2.5000000000000001E-3</v>
       </c>
       <c r="D6">
         <v>10619.1</v>
@@ -532,12 +1476,15 @@
         <v>8100</v>
       </c>
       <c r="C7">
-        <f>1/(25*60)</f>
-        <v>6.6666666666666664E-4</v>
+        <f>3/(25*60)</f>
+        <v>2E-3</v>
       </c>
       <c r="D7">
         <v>12749.44</v>
       </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C9" s="1"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D16">
@@ -545,5 +1492,6 @@
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Forgot to update curing calculations data from last commit
</commit_message>
<xml_diff>
--- a/Curing Calculations Data.xlsx
+++ b/Curing Calculations Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yushrajkapoor/Desktop/NauenLab/GELxy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{761A6A5E-C598-C94F-BAA8-06A82CAAF557}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C3858E3-AAA8-CB4A-B195-50D517755283}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8440" yWindow="760" windowWidth="26120" windowHeight="21580" xr2:uid="{EB474C7A-A58E-EB45-A49F-20C7A37E07CB}"/>
   </bookViews>
@@ -203,26 +203,23 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$7</c:f>
+              <c:f>Sheet1!$C$2:$C$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>9999</c:v>
+                  <c:v>0.01</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.01</c:v>
+                  <c:v>5.0000000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.0000000000000001E-3</c:v>
+                  <c:v>3.3333333333333335E-3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.3333333333333335E-3</c:v>
+                  <c:v>2.5000000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.5000000000000001E-3</c:v>
-                </c:pt>
-                <c:pt idx="5">
                   <c:v>2E-3</c:v>
                 </c:pt>
               </c:numCache>
@@ -230,26 +227,23 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$D$2:$D$7</c:f>
+              <c:f>Sheet1!$D$2:$D$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>2755.13</c:v>
+                  <c:v>4431.4399999999996</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4431.4399999999996</c:v>
+                  <c:v>7661.76</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7661.76</c:v>
+                  <c:v>8860.2000000000007</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8860.2000000000007</c:v>
+                  <c:v>10619.1</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>10619.1</c:v>
-                </c:pt>
-                <c:pt idx="5">
                   <c:v>12749.44</c:v>
                 </c:pt>
               </c:numCache>
@@ -1366,7 +1360,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A2" sqref="A2:D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1402,10 +1396,11 @@
         <v>8100</v>
       </c>
       <c r="C2">
-        <v>9999</v>
+        <f>3/(5*60)</f>
+        <v>0.01</v>
       </c>
       <c r="D2">
-        <v>2755.13</v>
+        <v>4431.4399999999996</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -1416,11 +1411,11 @@
         <v>8100</v>
       </c>
       <c r="C3">
-        <f>3/(5*60)</f>
-        <v>0.01</v>
+        <f>3/(10*60)</f>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="D3">
-        <v>4431.4399999999996</v>
+        <v>7661.76</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -1431,11 +1426,11 @@
         <v>8100</v>
       </c>
       <c r="C4">
-        <f>3/(10*60)</f>
-        <v>5.0000000000000001E-3</v>
+        <f>3/(15*60)</f>
+        <v>3.3333333333333335E-3</v>
       </c>
       <c r="D4">
-        <v>7661.76</v>
+        <v>8860.2000000000007</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -1446,11 +1441,11 @@
         <v>8100</v>
       </c>
       <c r="C5">
-        <f>3/(15*60)</f>
-        <v>3.3333333333333335E-3</v>
+        <f>3/(20*60)</f>
+        <v>2.5000000000000001E-3</v>
       </c>
       <c r="D5">
-        <v>8860.2000000000007</v>
+        <v>10619.1</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -1461,25 +1456,10 @@
         <v>8100</v>
       </c>
       <c r="C6">
-        <f>3/(20*60)</f>
-        <v>2.5000000000000001E-3</v>
-      </c>
-      <c r="D6">
-        <v>10619.1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>3</v>
-      </c>
-      <c r="B7">
-        <v>8100</v>
-      </c>
-      <c r="C7">
         <f>3/(25*60)</f>
         <v>2E-3</v>
       </c>
-      <c r="D7">
+      <c r="D6">
         <v>12749.44</v>
       </c>
     </row>

</xml_diff>